<commit_message>
Update Rizka - Lupa Kata Sandi (Btn MasukatauDaftar can't be detected)
</commit_message>
<xml_diff>
--- a/LupaKataSandi.xlsx
+++ b/LupaKataSandi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA900D5E-A083-4EC1-94AD-6A987C7D984C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B824E-757D-450C-AD6D-27BF6EF796B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{20144473-86DB-4B29-B5D0-6DB4014EC363}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{20144473-86DB-4B29-B5D0-6DB4014EC363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>email</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>A12345</t>
+  </si>
+  <si>
+    <t>emailSalah</t>
+  </si>
+  <si>
+    <t>lalalala</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +725,16 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -735,8 +750,9 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{1538F84E-4184-4761-B884-D6F0E3C20B97}"/>
     <hyperlink ref="A6" r:id="rId4" xr:uid="{CF3E3816-4ACE-4C13-8E84-3118D4890F86}"/>
     <hyperlink ref="A10" r:id="rId5" xr:uid="{78062C1C-84A0-479F-B87F-B12CF0C1FE8A}"/>
+    <hyperlink ref="A11" r:id="rId6" display="rizkariz20@gmail.com" xr:uid="{582E9C68-5448-4AF3-93F8-49AC789F7A71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - Data Ketinggalan Lupa Kata Sandi
</commit_message>
<xml_diff>
--- a/LupaKataSandi.xlsx
+++ b/LupaKataSandi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6FAF9D-E2A7-4C2C-874B-C6AFC1EE0A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4DA8B1-5B4E-4C4D-83F7-FEB901DF595D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{20144473-86DB-4B29-B5D0-6DB4014EC363}"/>
+    <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{20144473-86DB-4B29-B5D0-6DB4014EC363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Lupa Kata Sandi - Data bind updated.
</commit_message>
<xml_diff>
--- a/LupaKataSandi.xlsx
+++ b/LupaKataSandi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD4A2AE-115D-4B12-8BCF-5D5A433A54F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B1A3AB-819A-4792-A45E-D38886006413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{20144473-86DB-4B29-B5D0-6DB4014EC363}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="32">
   <si>
     <t>email</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>passwordTidakSesuaiHarusDiisi</t>
+  </si>
+  <si>
+    <t>emailKosong</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,6 +465,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -778,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EFA2CD0-E11E-48A2-AA8F-B59900E87E0F}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,9 +843,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="27">
-        <v>261294</v>
-      </c>
+      <c r="C3" s="32"/>
       <c r="D3" s="21"/>
       <c r="E3" s="19"/>
       <c r="F3" s="24" t="s">
@@ -847,19 +851,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="23">
-        <v>444444</v>
-      </c>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="21"/>
       <c r="E4" s="19"/>
       <c r="F4" s="24" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -869,13 +867,13 @@
       <c r="B5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="22">
-        <v>261294</v>
+      <c r="C5" s="23">
+        <v>444444</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="19"/>
       <c r="F5" s="24" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,12 +886,10 @@
       <c r="C6" s="22">
         <v>261294</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="D6" s="21"/>
       <c r="E6" s="19"/>
       <c r="F6" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -906,12 +902,12 @@
       <c r="C7" s="22">
         <v>261294</v>
       </c>
-      <c r="D7" s="21">
-        <v>1234567</v>
+      <c r="D7" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -924,12 +920,12 @@
       <c r="C8" s="22">
         <v>261294</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>9</v>
+      <c r="D8" s="21">
+        <v>1234567</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,13 +939,11 @@
         <v>261294</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>27</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E9" s="19"/>
       <c r="F9" s="24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -965,8 +959,28 @@
       <c r="D10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="19"/>
+      <c r="E10" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="F10" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="22">
+        <v>261294</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="24" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>